<commit_message>
afb, ffi, y ranking de enfermedades
</commit_message>
<xml_diff>
--- a/survey/Manejo de Guacheras Encuesta.xlsx
+++ b/survey/Manejo de Guacheras Encuesta.xlsx
@@ -5562,63 +5562,6 @@
       </c>
       <c r="Q102"/>
     </row>
-    <row r="103">
-      <c r="A103"/>
-      <c r="B103"/>
-      <c r="C103"/>
-      <c r="D103"/>
-      <c r="E103"/>
-      <c r="F103"/>
-      <c r="G103"/>
-      <c r="H103"/>
-      <c r="I103"/>
-      <c r="J103"/>
-      <c r="K103"/>
-      <c r="L103"/>
-      <c r="M103"/>
-      <c r="N103"/>
-      <c r="O103"/>
-      <c r="P103"/>
-      <c r="Q103"/>
-    </row>
-    <row r="104">
-      <c r="A104"/>
-      <c r="B104"/>
-      <c r="C104"/>
-      <c r="D104"/>
-      <c r="E104"/>
-      <c r="F104"/>
-      <c r="G104"/>
-      <c r="H104"/>
-      <c r="I104"/>
-      <c r="J104"/>
-      <c r="K104"/>
-      <c r="L104"/>
-      <c r="M104"/>
-      <c r="N104"/>
-      <c r="O104"/>
-      <c r="P104"/>
-      <c r="Q104"/>
-    </row>
-    <row r="105">
-      <c r="A105"/>
-      <c r="B105"/>
-      <c r="C105"/>
-      <c r="D105"/>
-      <c r="E105"/>
-      <c r="F105"/>
-      <c r="G105"/>
-      <c r="H105"/>
-      <c r="I105"/>
-      <c r="J105"/>
-      <c r="K105"/>
-      <c r="L105"/>
-      <c r="M105"/>
-      <c r="N105"/>
-      <c r="O105"/>
-      <c r="P105"/>
-      <c r="Q105"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>